<commit_message>
MTP089 done now with EUVM joint obs included
</commit_message>
<xml_diff>
--- a/observations/orbit_plans/mtp089/nomad_mtp089_plan.xlsx
+++ b/observations/orbit_plans/mtp089/nomad_mtp089_plan.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\orbit_plans\mtp089\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF1C5A-0F71-4C4B-AF80-B2C353279961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2976" yWindow="1704" windowWidth="30960" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1693,8 +1699,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1731,13 +1737,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1775,7 +1789,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1809,6 +1823,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1843,9 +1858,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2018,14 +2034,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2066,7 +2087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2083,7 +2104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2106,7 +2127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2138,7 +2159,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2170,7 +2191,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2202,7 +2223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2234,7 +2255,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2251,7 +2272,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2283,7 +2304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2315,7 +2336,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2347,7 +2368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2379,7 +2400,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2402,7 +2423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -2416,7 +2437,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2430,7 +2451,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2462,7 +2483,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2494,7 +2515,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2508,7 +2529,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2543,7 +2564,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2554,7 +2575,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>14</v>
       </c>
@@ -2568,7 +2589,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
@@ -2585,7 +2606,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2599,10 +2620,10 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
@@ -2617,7 +2638,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>14</v>
       </c>
@@ -2631,7 +2652,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2645,10 +2666,10 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G25" t="s">
         <v>6</v>
@@ -2666,7 +2687,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2689,7 +2710,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>14</v>
       </c>
@@ -2703,7 +2724,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>14</v>
       </c>
@@ -2717,7 +2738,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2749,7 +2770,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>14</v>
       </c>
@@ -2763,7 +2784,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2795,7 +2816,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2818,7 +2839,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -2829,7 +2850,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>14</v>
       </c>
@@ -2843,7 +2864,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2875,7 +2896,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>14</v>
       </c>
@@ -2889,7 +2910,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2921,7 +2942,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2953,7 +2974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2970,7 +2991,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2993,7 +3014,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>14</v>
       </c>
@@ -3007,7 +3028,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3036,7 +3057,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>47</v>
       </c>
@@ -3050,7 +3071,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>14</v>
       </c>
@@ -3064,7 +3085,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3087,7 +3108,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3119,7 +3140,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>7</v>
       </c>
@@ -3136,7 +3157,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3168,7 +3189,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>3</v>
       </c>
@@ -3185,7 +3206,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -3208,7 +3229,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>14</v>
       </c>
@@ -3222,7 +3243,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1</v>
       </c>
@@ -3254,7 +3275,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1</v>
       </c>
@@ -3277,7 +3298,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>14</v>
       </c>
@@ -3288,7 +3309,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>47</v>
       </c>
@@ -3302,7 +3323,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1</v>
       </c>
@@ -3334,7 +3355,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>14</v>
       </c>
@@ -3348,7 +3369,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1</v>
       </c>
@@ -3380,7 +3401,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -3412,7 +3433,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>14</v>
       </c>
@@ -3426,7 +3447,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
@@ -3458,7 +3479,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3</v>
       </c>
@@ -3475,7 +3496,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1</v>
       </c>
@@ -3498,7 +3519,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>14</v>
       </c>
@@ -3512,7 +3533,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>14</v>
       </c>
@@ -3526,7 +3547,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1</v>
       </c>
@@ -3558,7 +3579,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>14</v>
       </c>
@@ -3572,7 +3593,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1</v>
       </c>
@@ -3604,7 +3625,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>14</v>
       </c>
@@ -3618,7 +3639,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1</v>
       </c>
@@ -3650,7 +3671,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1</v>
       </c>
@@ -3682,7 +3703,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>14</v>
       </c>
@@ -3696,7 +3717,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1</v>
       </c>
@@ -3728,7 +3749,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>14</v>
       </c>
@@ -3742,7 +3763,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -3765,7 +3786,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3</v>
       </c>
@@ -3782,7 +3803,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1</v>
       </c>
@@ -3814,7 +3835,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1</v>
       </c>
@@ -3837,7 +3858,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>3</v>
       </c>
@@ -3851,7 +3872,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1</v>
       </c>
@@ -3883,7 +3904,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>14</v>
       </c>
@@ -3897,7 +3918,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1</v>
       </c>
@@ -3929,7 +3950,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1</v>
       </c>
@@ -3964,7 +3985,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>14</v>
       </c>
@@ -3978,7 +3999,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1</v>
       </c>
@@ -4010,7 +4031,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>14</v>
       </c>
@@ -4021,7 +4042,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>14</v>
       </c>
@@ -4032,7 +4053,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>3</v>
       </c>
@@ -4046,7 +4067,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1</v>
       </c>
@@ -4078,7 +4099,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1</v>
       </c>
@@ -4104,7 +4125,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>14</v>
       </c>
@@ -4118,7 +4139,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1</v>
       </c>
@@ -4150,7 +4171,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>14</v>
       </c>
@@ -4164,7 +4185,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1</v>
       </c>
@@ -4196,7 +4217,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>3</v>
       </c>
@@ -4210,7 +4231,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1</v>
       </c>
@@ -4242,7 +4263,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1</v>
       </c>
@@ -4274,7 +4295,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>3</v>
       </c>
@@ -4288,7 +4309,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1</v>
       </c>
@@ -4320,7 +4341,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>3</v>
       </c>
@@ -4334,7 +4355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1</v>
       </c>
@@ -4366,7 +4387,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>14</v>
       </c>
@@ -4380,7 +4401,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1</v>
       </c>
@@ -4412,7 +4433,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1</v>
       </c>
@@ -4444,7 +4465,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>3</v>
       </c>
@@ -4461,7 +4482,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1</v>
       </c>
@@ -4493,7 +4514,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>14</v>
       </c>
@@ -4507,7 +4528,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1</v>
       </c>
@@ -4539,7 +4560,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1</v>
       </c>
@@ -4574,7 +4595,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>14</v>
       </c>
@@ -4588,7 +4609,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1</v>
       </c>
@@ -4620,7 +4641,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>14</v>
       </c>
@@ -4634,7 +4655,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>1</v>
       </c>
@@ -4657,7 +4678,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>1</v>
       </c>
@@ -4689,7 +4710,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>3</v>
       </c>
@@ -4706,7 +4727,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1</v>
       </c>
@@ -4738,7 +4759,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>14</v>
       </c>
@@ -4752,7 +4773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>1</v>
       </c>
@@ -4784,7 +4805,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>3</v>
       </c>
@@ -4801,7 +4822,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>1</v>
       </c>
@@ -4833,7 +4854,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>1</v>
       </c>
@@ -4868,7 +4889,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>3</v>
       </c>
@@ -4885,7 +4906,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>1</v>
       </c>
@@ -4920,7 +4941,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>14</v>
       </c>
@@ -4934,7 +4955,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>1</v>
       </c>
@@ -4957,7 +4978,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>3</v>
       </c>
@@ -4974,7 +4995,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>14</v>
       </c>
@@ -4988,7 +5009,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>1</v>
       </c>
@@ -5020,7 +5041,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>3</v>
       </c>
@@ -5037,7 +5058,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>1</v>
       </c>
@@ -5069,7 +5090,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>3</v>
       </c>
@@ -5086,7 +5107,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>1</v>
       </c>
@@ -5118,7 +5139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>1</v>
       </c>
@@ -5150,7 +5171,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>3</v>
       </c>
@@ -5167,7 +5188,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>1</v>
       </c>
@@ -5202,7 +5223,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>14</v>
       </c>
@@ -5216,7 +5237,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>1</v>
       </c>
@@ -5248,7 +5269,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>1</v>
       </c>
@@ -5271,7 +5292,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>3</v>
       </c>
@@ -5288,7 +5309,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>1</v>
       </c>
@@ -5311,7 +5332,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>14</v>
       </c>
@@ -5325,7 +5346,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>1</v>
       </c>
@@ -5357,7 +5378,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>3</v>
       </c>
@@ -5374,7 +5395,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>1</v>
       </c>
@@ -5406,7 +5427,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>1</v>
       </c>
@@ -5438,7 +5459,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>14</v>
       </c>
@@ -5452,7 +5473,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>1</v>
       </c>
@@ -5487,7 +5508,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>14</v>
       </c>
@@ -5501,7 +5522,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>1</v>
       </c>
@@ -5533,7 +5554,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>3</v>
       </c>
@@ -5550,7 +5571,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>1</v>
       </c>
@@ -5582,7 +5603,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>1</v>
       </c>
@@ -5605,7 +5626,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>14</v>
       </c>
@@ -5619,7 +5640,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>1</v>
       </c>
@@ -5651,7 +5672,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>14</v>
       </c>
@@ -5665,7 +5686,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>1</v>
       </c>
@@ -5697,7 +5718,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>14</v>
       </c>
@@ -5708,7 +5729,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>14</v>
       </c>
@@ -5722,7 +5743,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>1</v>
       </c>
@@ -5754,7 +5775,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>14</v>
       </c>
@@ -5768,7 +5789,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>1</v>
       </c>
@@ -5800,7 +5821,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>14</v>
       </c>
@@ -5814,7 +5835,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>1</v>
       </c>
@@ -5843,7 +5864,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>47</v>
       </c>
@@ -5857,7 +5878,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>1</v>
       </c>
@@ -5880,7 +5901,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>3</v>
       </c>
@@ -5897,7 +5918,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>1</v>
       </c>
@@ -5929,7 +5950,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>14</v>
       </c>
@@ -5943,7 +5964,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>28</v>
       </c>
@@ -5966,7 +5987,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>14</v>
       </c>
@@ -5980,7 +6001,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>1</v>
       </c>
@@ -6015,7 +6036,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>14</v>
       </c>
@@ -6026,7 +6047,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>14</v>
       </c>
@@ -6037,7 +6058,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>1</v>
       </c>
@@ -6069,7 +6090,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>14</v>
       </c>
@@ -6083,7 +6104,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>1</v>
       </c>
@@ -6115,7 +6136,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>14</v>
       </c>
@@ -6129,7 +6150,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>1</v>
       </c>
@@ -6161,7 +6182,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>14</v>
       </c>
@@ -6175,7 +6196,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>1</v>
       </c>
@@ -6207,7 +6228,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>1</v>
       </c>
@@ -6236,7 +6257,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>47</v>
       </c>
@@ -6250,7 +6271,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>14</v>
       </c>
@@ -6264,7 +6285,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>1</v>
       </c>
@@ -6296,7 +6317,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>14</v>
       </c>
@@ -6310,7 +6331,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>1</v>
       </c>
@@ -6342,7 +6363,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>1</v>
       </c>
@@ -6368,7 +6389,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>14</v>
       </c>
@@ -6382,7 +6403,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>1</v>
       </c>
@@ -6414,7 +6435,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>3</v>
       </c>
@@ -6431,7 +6452,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>1</v>
       </c>
@@ -6463,7 +6484,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>1</v>
       </c>
@@ -6495,7 +6516,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>14</v>
       </c>
@@ -6509,7 +6530,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>1</v>
       </c>
@@ -6541,7 +6562,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>14</v>
       </c>
@@ -6555,7 +6576,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>1</v>
       </c>
@@ -6587,7 +6608,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>14</v>
       </c>
@@ -6601,7 +6622,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>1</v>
       </c>
@@ -6633,7 +6654,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>1</v>
       </c>
@@ -6665,7 +6686,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>14</v>
       </c>
@@ -6679,7 +6700,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>14</v>
       </c>
@@ -6693,7 +6714,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>1</v>
       </c>
@@ -6716,7 +6737,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>14</v>
       </c>
@@ -6730,7 +6751,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>1</v>
       </c>
@@ -6765,7 +6786,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>14</v>
       </c>
@@ -6776,7 +6797,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>47</v>
       </c>
@@ -6790,7 +6811,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>1</v>
       </c>
@@ -6822,7 +6843,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>1</v>
       </c>
@@ -6857,7 +6878,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>14</v>
       </c>
@@ -6871,7 +6892,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>1</v>
       </c>
@@ -6903,7 +6924,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>14</v>
       </c>
@@ -6917,7 +6938,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>14</v>
       </c>
@@ -6931,7 +6952,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>1</v>
       </c>
@@ -6963,7 +6984,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>1</v>
       </c>
@@ -6986,7 +7007,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>14</v>
       </c>
@@ -7000,7 +7021,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>1</v>
       </c>
@@ -7032,7 +7053,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>14</v>
       </c>
@@ -7046,7 +7067,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>3</v>
       </c>
@@ -7063,7 +7084,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>1</v>
       </c>
@@ -7095,7 +7116,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>1</v>
       </c>
@@ -7127,7 +7148,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>14</v>
       </c>
@@ -7141,7 +7162,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>1</v>
       </c>
@@ -7173,7 +7194,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>14</v>
       </c>
@@ -7184,7 +7205,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>47</v>
       </c>
@@ -7198,7 +7219,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>1</v>
       </c>
@@ -7221,7 +7242,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>14</v>
       </c>
@@ -7235,7 +7256,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>1</v>
       </c>
@@ -7258,7 +7279,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>1</v>
       </c>
@@ -7290,7 +7311,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>14</v>
       </c>
@@ -7304,7 +7325,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>3</v>
       </c>
@@ -7321,7 +7342,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>1</v>
       </c>
@@ -7353,7 +7374,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>14</v>
       </c>
@@ -7367,7 +7388,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="233" spans="1:13">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>1</v>
       </c>
@@ -7399,7 +7420,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>14</v>
       </c>
@@ -7413,7 +7434,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>1</v>
       </c>
@@ -7445,7 +7466,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="236" spans="1:13">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>14</v>
       </c>
@@ -7459,7 +7480,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>1</v>
       </c>
@@ -7482,7 +7503,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="238" spans="1:13">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>14</v>
       </c>
@@ -7496,7 +7517,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="239" spans="1:13">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>1</v>
       </c>
@@ -7522,7 +7543,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>14</v>
       </c>
@@ -7536,7 +7557,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>1</v>
       </c>
@@ -7568,7 +7589,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>14</v>
       </c>
@@ -7582,7 +7603,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>1</v>
       </c>
@@ -7614,7 +7635,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>14</v>
       </c>
@@ -7628,7 +7649,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>1</v>
       </c>
@@ -7651,7 +7672,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>14</v>
       </c>
@@ -7665,7 +7686,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>1</v>
       </c>
@@ -7688,7 +7709,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>1</v>
       </c>
@@ -7711,7 +7732,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>14</v>
       </c>
@@ -7725,7 +7746,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>1</v>
       </c>
@@ -7748,7 +7769,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>3</v>
       </c>
@@ -7765,7 +7786,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>1</v>
       </c>
@@ -7788,7 +7809,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>14</v>
       </c>
@@ -7799,7 +7820,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>14</v>
       </c>
@@ -7810,7 +7831,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>1</v>
       </c>
@@ -7833,7 +7854,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>1</v>
       </c>
@@ -7856,7 +7877,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="257" spans="1:13">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>14</v>
       </c>
@@ -7867,7 +7888,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>14</v>
       </c>
@@ -7878,7 +7899,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>14</v>
       </c>
@@ -7892,7 +7913,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="260" spans="1:13">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>14</v>
       </c>
@@ -7906,7 +7927,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>1</v>
       </c>
@@ -7929,7 +7950,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="262" spans="1:13">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>14</v>
       </c>
@@ -7943,7 +7964,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="263" spans="1:13">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>1</v>
       </c>
@@ -7969,7 +7990,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="264" spans="1:13">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>14</v>
       </c>
@@ -7983,7 +8004,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="265" spans="1:13">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>1</v>
       </c>
@@ -8006,7 +8027,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="266" spans="1:13">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>1</v>
       </c>
@@ -8029,7 +8050,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="267" spans="1:13">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>14</v>
       </c>
@@ -8043,7 +8064,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="268" spans="1:13">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>1</v>
       </c>
@@ -8066,7 +8087,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="269" spans="1:13">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>14</v>
       </c>
@@ -8080,7 +8101,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="270" spans="1:13">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>1</v>
       </c>
@@ -8103,7 +8124,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="271" spans="1:13">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>1</v>
       </c>
@@ -8126,7 +8147,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="272" spans="1:13">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>14</v>
       </c>
@@ -8140,7 +8161,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="273" spans="1:13">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>1</v>
       </c>
@@ -8163,7 +8184,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>14</v>
       </c>
@@ -8177,7 +8198,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="275" spans="1:13">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>1</v>
       </c>
@@ -8200,7 +8221,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>1</v>
       </c>
@@ -8226,7 +8247,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>14</v>
       </c>
@@ -8240,7 +8261,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="278" spans="1:13">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>14</v>
       </c>
@@ -8254,7 +8275,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="279" spans="1:13">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>1</v>
       </c>
@@ -8277,7 +8298,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="280" spans="1:13">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>14</v>
       </c>
@@ -8291,7 +8312,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="281" spans="1:13">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>1</v>
       </c>
@@ -8314,7 +8335,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="282" spans="1:13">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>14</v>
       </c>
@@ -8328,7 +8349,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>1</v>
       </c>
@@ -8351,7 +8372,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="284" spans="1:13">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>1</v>
       </c>
@@ -8374,7 +8395,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="285" spans="1:13">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>3</v>
       </c>
@@ -8391,7 +8412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="286" spans="1:13">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>1</v>
       </c>
@@ -8414,7 +8435,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="287" spans="1:13">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>14</v>
       </c>
@@ -8428,7 +8449,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="288" spans="1:13">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>1</v>
       </c>
@@ -8451,7 +8472,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="289" spans="1:13">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>14</v>
       </c>
@@ -8465,7 +8486,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="290" spans="1:13">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>1</v>
       </c>
@@ -8488,7 +8509,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="291" spans="1:13">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>1</v>
       </c>
@@ -8511,7 +8532,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="292" spans="1:13">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>14</v>
       </c>
@@ -8525,7 +8546,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="293" spans="1:13">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>1</v>
       </c>
@@ -8548,7 +8569,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="294" spans="1:13">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>14</v>
       </c>
@@ -8562,7 +8583,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="295" spans="1:13">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>1</v>
       </c>
@@ -8588,7 +8609,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="296" spans="1:13">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>1</v>
       </c>
@@ -8611,7 +8632,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="297" spans="1:13">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>14</v>
       </c>
@@ -8625,7 +8646,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="298" spans="1:13">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>1</v>
       </c>
@@ -8648,7 +8669,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="299" spans="1:13">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>14</v>
       </c>
@@ -8659,7 +8680,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="300" spans="1:13">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>14</v>
       </c>
@@ -8670,7 +8691,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="301" spans="1:13">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>1</v>
       </c>
@@ -8693,7 +8714,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="302" spans="1:13">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>1</v>
       </c>
@@ -8716,7 +8737,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="303" spans="1:13">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>14</v>
       </c>
@@ -8730,7 +8751,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="304" spans="1:13">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>1</v>
       </c>
@@ -8756,7 +8777,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="305" spans="1:13">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>14</v>
       </c>
@@ -8770,7 +8791,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="306" spans="1:13">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>1</v>
       </c>
@@ -8793,7 +8814,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="307" spans="1:13">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>3</v>
       </c>
@@ -8810,7 +8831,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="308" spans="1:13">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>1</v>
       </c>
@@ -8830,7 +8851,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="309" spans="1:13">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>47</v>
       </c>
@@ -8844,7 +8865,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="310" spans="1:13">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>1</v>
       </c>
@@ -8867,7 +8888,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="311" spans="1:13">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>14</v>
       </c>
@@ -8881,7 +8902,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="312" spans="1:13">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>14</v>
       </c>
@@ -8895,7 +8916,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="313" spans="1:13">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>1</v>
       </c>
@@ -8918,7 +8939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:13">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>14</v>
       </c>
@@ -8932,7 +8953,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="315" spans="1:13">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>1</v>
       </c>
@@ -8955,7 +8976,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="316" spans="1:13">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>3</v>
       </c>
@@ -8972,7 +8993,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="317" spans="1:13">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>1</v>
       </c>
@@ -8995,7 +9016,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="318" spans="1:13">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>1</v>
       </c>
@@ -9018,7 +9039,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="319" spans="1:13">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>14</v>
       </c>
@@ -9032,7 +9053,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="320" spans="1:13">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>1</v>
       </c>
@@ -9052,7 +9073,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="321" spans="1:13">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>47</v>
       </c>
@@ -9066,7 +9087,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="322" spans="1:13">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>14</v>
       </c>
@@ -9080,7 +9101,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="323" spans="1:13">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>1</v>
       </c>
@@ -9103,7 +9124,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="324" spans="1:13">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>14</v>
       </c>
@@ -9117,7 +9138,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="325" spans="1:13">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>1</v>
       </c>
@@ -9140,7 +9161,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="326" spans="1:13">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>3</v>
       </c>
@@ -9157,7 +9178,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="327" spans="1:13">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>14</v>
       </c>
@@ -9171,7 +9192,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="328" spans="1:13">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>1</v>
       </c>
@@ -9194,7 +9215,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="329" spans="1:13">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>14</v>
       </c>
@@ -9208,7 +9229,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="330" spans="1:13">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>1</v>
       </c>
@@ -9228,7 +9249,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="331" spans="1:13">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>14</v>
       </c>
@@ -9239,7 +9260,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="332" spans="1:13">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>1</v>
       </c>
@@ -9262,7 +9283,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="333" spans="1:13">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>14</v>
       </c>
@@ -9276,7 +9297,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="334" spans="1:13">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>1</v>
       </c>
@@ -9302,7 +9323,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="335" spans="1:13">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>14</v>
       </c>
@@ -9316,7 +9337,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="336" spans="1:13">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>1</v>
       </c>
@@ -9339,7 +9360,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="337" spans="1:13">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>14</v>
       </c>
@@ -9353,7 +9374,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="338" spans="1:13">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>3</v>
       </c>
@@ -9370,7 +9391,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="339" spans="1:13">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>1</v>
       </c>
@@ -9393,7 +9414,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="340" spans="1:13">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>1</v>
       </c>
@@ -9416,7 +9437,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="341" spans="1:13">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>14</v>
       </c>
@@ -9430,7 +9451,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="342" spans="1:13">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>1</v>
       </c>

</xml_diff>